<commit_message>
Deck Creator, Assets, Excel db
title
</commit_message>
<xml_diff>
--- a/Transcendence/Assets/notes/data-set.xlsx
+++ b/Transcendence/Assets/notes/data-set.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Transcendence\Transcendence\Transcendence\Assets\notes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
   </bookViews>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="204">
   <si>
     <t>name</t>
   </si>
@@ -237,13 +242,412 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Hawkblade Honor Guard</t>
+  </si>
+  <si>
+    <t>Citadel</t>
+  </si>
+  <si>
+    <t>Shadow Orb</t>
+  </si>
+  <si>
+    <t>Deals 3 damage to 2 targets, chance to inflict fear</t>
+  </si>
+  <si>
+    <t>Swap</t>
+  </si>
+  <si>
+    <t>Swaps the positions of 2 allied creatures</t>
+  </si>
+  <si>
+    <t>Friendly Creature</t>
+  </si>
+  <si>
+    <t>Skeletal Construct</t>
+  </si>
+  <si>
+    <t>Pious Zealot</t>
+  </si>
+  <si>
+    <t>Temple</t>
+  </si>
+  <si>
+    <t>Exemplar of Radiance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athaliah, the Revered Adjudicator </t>
+  </si>
+  <si>
+    <t>Razark, Eradicator of the Meek</t>
+  </si>
+  <si>
+    <t>Hollow Faceeater</t>
+  </si>
+  <si>
+    <t>Fallen Angel</t>
+  </si>
+  <si>
+    <t>Darkruin Gargoyle</t>
+  </si>
+  <si>
+    <t>Tortured Soul</t>
+  </si>
+  <si>
+    <t>Lightwhisper Monk</t>
+  </si>
+  <si>
+    <t>Lightwhisper Guardian</t>
+  </si>
+  <si>
+    <t>Vampire Servant</t>
+  </si>
+  <si>
+    <t>Baron Godfrey</t>
+  </si>
+  <si>
+    <t>Mindless Bloodseeker</t>
+  </si>
+  <si>
+    <t>Battlelord</t>
+  </si>
+  <si>
+    <t>Warpriest</t>
+  </si>
+  <si>
+    <t>Darkruin Sentry</t>
+  </si>
+  <si>
+    <t>Shadewood Stalker</t>
+  </si>
+  <si>
+    <t>Bloodsated Slayer</t>
+  </si>
+  <si>
+    <t>Sunbathed Cleric</t>
+  </si>
+  <si>
+    <t>Silver Covenant Acolyte</t>
+  </si>
+  <si>
+    <t>Hawkblade Crossbowman</t>
+  </si>
+  <si>
+    <t>Lightstep Archer</t>
+  </si>
+  <si>
+    <t>Guardian Angel</t>
+  </si>
+  <si>
+    <t>Lightstep Warden</t>
+  </si>
+  <si>
+    <t>Silver Covenant Priest</t>
+  </si>
+  <si>
+    <t>Duskmire Huntress</t>
+  </si>
+  <si>
+    <t>Blood Ritual</t>
+  </si>
+  <si>
+    <t>Deals 2 damage to all friendly creatures on a node, then deals that damage to an enemy target</t>
+  </si>
+  <si>
+    <t>Boon</t>
+  </si>
+  <si>
+    <t>Divine Omen</t>
+  </si>
+  <si>
+    <t>Drains all remaining mana (x), heals creature for 2 damage at the end of each round for x rounds</t>
+  </si>
+  <si>
+    <t>Inspire</t>
+  </si>
+  <si>
+    <t>Gives friendly creatures +2 attack for 1 turn</t>
+  </si>
+  <si>
+    <t>Hallowed Ground</t>
+  </si>
+  <si>
+    <t>No new enemy creatures can enter target node during daytime for 3 rounds</t>
+  </si>
+  <si>
+    <t>Sun Corona</t>
+  </si>
+  <si>
+    <t>Deals 4 damage to all enemy creatures on target node. Can only be used during day.</t>
+  </si>
+  <si>
+    <t>Divine Blessing</t>
+  </si>
+  <si>
+    <t>Target friendly creature gains +2/+3</t>
+  </si>
+  <si>
+    <t>Rally</t>
+  </si>
+  <si>
+    <t>Draws the next two creatures in your deck</t>
+  </si>
+  <si>
+    <t>Purify</t>
+  </si>
+  <si>
+    <t>Removes all debuffs from target creature.</t>
+  </si>
+  <si>
+    <t>Smite</t>
+  </si>
+  <si>
+    <t>Deals 6 damage.</t>
+  </si>
+  <si>
+    <t>Elusive</t>
+  </si>
+  <si>
+    <t>Friendly creature's next attack ignores guards.</t>
+  </si>
+  <si>
+    <t>Drain Soul</t>
+  </si>
+  <si>
+    <t>Deals 4 damage, heals friendly creature for 2.</t>
+  </si>
+  <si>
+    <t>Tides of Chaos</t>
+  </si>
+  <si>
+    <t>Enemy creatures in target node take 2 damage during nighttime for 5 rounds</t>
+  </si>
+  <si>
+    <t>Shadow Barrage</t>
+  </si>
+  <si>
+    <t>Deals 6 damage to all enemies in node.</t>
+  </si>
+  <si>
+    <t>Chain Spirit</t>
+  </si>
+  <si>
+    <t>Target creature cannot be brought below 1 hp this round.</t>
+  </si>
+  <si>
+    <t>Delirium</t>
+  </si>
+  <si>
+    <t>Target creature cannot attune and has a 0.33 chance to attack the wrong enemy for 2 rounds.</t>
+  </si>
+  <si>
+    <t>Fiendish Resilience</t>
+  </si>
+  <si>
+    <t>Beguiling Strike</t>
+  </si>
+  <si>
+    <t>Target creature's next attack inflicts fear.</t>
+  </si>
+  <si>
+    <t>Thristing Spear</t>
+  </si>
+  <si>
+    <t>Death Whisper</t>
+  </si>
+  <si>
+    <t>Target creature takes 8 damage if isolated, or half that if in a group.</t>
+  </si>
+  <si>
+    <t>Fleshmelting Bolt</t>
+  </si>
+  <si>
+    <t>Deals 3 damage for 3 rounds.</t>
+  </si>
+  <si>
+    <t>Fireball</t>
+  </si>
+  <si>
+    <t>Deals 8 damage.</t>
+  </si>
+  <si>
+    <t>Grim Transformation</t>
+  </si>
+  <si>
+    <t>Target friendly creature gains +3/+2</t>
+  </si>
+  <si>
+    <t>Mending Touch</t>
+  </si>
+  <si>
+    <t>Bane</t>
+  </si>
+  <si>
+    <t>Deals 2 damage.</t>
+  </si>
+  <si>
+    <t>Fear</t>
+  </si>
+  <si>
+    <t>Deals 1 damage and inflicts fear.</t>
+  </si>
+  <si>
+    <t>Silence</t>
+  </si>
+  <si>
+    <t>Target creature is silenced.</t>
+  </si>
+  <si>
+    <t>Restoration</t>
+  </si>
+  <si>
+    <t>Target creature heals 3 health for 2 rounds.</t>
+  </si>
+  <si>
+    <t>Sacred Flame</t>
+  </si>
+  <si>
+    <t>Sanctuary</t>
+  </si>
+  <si>
+    <t>Friendly creatures in target node take no damage this round.</t>
+  </si>
+  <si>
+    <t>Clairvoyance</t>
+  </si>
+  <si>
+    <t>View the top 2 cards of your opponent's deck.</t>
+  </si>
+  <si>
+    <t>Cure Wounds</t>
+  </si>
+  <si>
+    <t>Heroism</t>
+  </si>
+  <si>
+    <t>Great Storm</t>
+  </si>
+  <si>
+    <t>Thunderwave</t>
+  </si>
+  <si>
+    <t>Earthquake</t>
+  </si>
+  <si>
+    <t>Daybreak</t>
+  </si>
+  <si>
+    <t>Changes time to Day</t>
+  </si>
+  <si>
+    <t>Shroud of Night</t>
+  </si>
+  <si>
+    <t>Changes time to Night</t>
+  </si>
+  <si>
+    <t>Wish</t>
+  </si>
+  <si>
+    <t>Hand of Death</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Banish</t>
+  </si>
+  <si>
+    <t>Target creature returns to your opponent's hand and costs 2 more (but not above 12).</t>
+  </si>
+  <si>
+    <t>Blight</t>
+  </si>
+  <si>
+    <t>Target creature is returned to your opponent</t>
+  </si>
+  <si>
+    <t>True Strike</t>
+  </si>
+  <si>
+    <t>Target creature's next attack deals double damage</t>
+  </si>
+  <si>
+    <t>Sunburst</t>
+  </si>
+  <si>
+    <t>A shining burst of 5 damage</t>
+  </si>
+  <si>
+    <t>Remain Vigilant</t>
+  </si>
+  <si>
+    <t>Target friendly creature guards</t>
+  </si>
+  <si>
+    <t>Form Ranks</t>
+  </si>
+  <si>
+    <t>All friendly creatures may move positions</t>
+  </si>
+  <si>
+    <t>Spells</t>
+  </si>
+  <si>
+    <t>Creatures</t>
+  </si>
+  <si>
+    <t>~15</t>
+  </si>
+  <si>
+    <t>~25</t>
+  </si>
+  <si>
+    <t>Boons</t>
+  </si>
+  <si>
+    <t>Lows</t>
+  </si>
+  <si>
+    <t>Mids</t>
+  </si>
+  <si>
+    <t>Highs</t>
+  </si>
+  <si>
+    <t>To Create</t>
+  </si>
+  <si>
+    <t>Hawkblade Apprentice</t>
+  </si>
+  <si>
+    <t>Umbrite</t>
+  </si>
+  <si>
+    <t>Sunkeeper</t>
+  </si>
+  <si>
+    <t>Brighteye Inquisitor</t>
+  </si>
+  <si>
+    <t>Brighteye Sister</t>
+  </si>
+  <si>
+    <t>Gloryseeker</t>
+  </si>
+  <si>
+    <t>Nathan Vaska</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +674,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -277,6 +682,15 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -294,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -358,11 +772,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -376,11 +803,381 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="91">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA08768"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA08768"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB1A0C7"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB1A0C7"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA08768"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA08768"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA08768"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA08768"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA08768"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA08768"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA08768"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1026,95 +1823,14 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA08768"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA08768"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1155,40 +1871,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L28" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:L28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L116" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:L116">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Citadel"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A30:L111">
+    <sortCondition sortBy="cellColor" ref="E1:E114" dxfId="15"/>
+  </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" uniqueName="name" name="name" dataDxfId="10">
+    <tableColumn id="1" uniqueName="name" name="name" dataDxfId="60">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ID" name="ID" dataDxfId="9">
+    <tableColumn id="2" uniqueName="ID" name="ID" dataDxfId="59">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@ID" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="description" name="description" dataDxfId="8">
+    <tableColumn id="3" uniqueName="description" name="description" dataDxfId="58">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="alliance" name="alliance" dataDxfId="7">
+    <tableColumn id="4" uniqueName="alliance" name="alliance" dataDxfId="57">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@alliance" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="type" name="type" dataDxfId="6">
+    <tableColumn id="5" uniqueName="type" name="type" dataDxfId="56">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="cost" name="cost" dataDxfId="5">
+    <tableColumn id="6" uniqueName="cost" name="cost" dataDxfId="55">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@cost" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="attack" name="attack" dataDxfId="4">
+    <tableColumn id="7" uniqueName="attack" name="attack" dataDxfId="54">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@attack" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="health" name="health" dataDxfId="3">
+    <tableColumn id="8" uniqueName="health" name="health" dataDxfId="53">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@health" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="defense" name="defense" dataDxfId="2">
+    <tableColumn id="9" uniqueName="defense" name="defense" dataDxfId="52">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@defense" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="range" name="range" dataDxfId="1">
+    <tableColumn id="10" uniqueName="range" name="range" dataDxfId="51">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@range" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="target" name="target" dataDxfId="0">
+    <tableColumn id="11" uniqueName="target" name="target" dataDxfId="50">
       <xmlColumnPr mapId="1" xpath="/data-set/card/@target" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="12" uniqueName="image" name="Column1"/>
@@ -1240,7 +1965,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1275,7 +2000,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1484,10 +2209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +2269,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1579,7 +2304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1614,7 +2339,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -1649,7 +2374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1684,7 +2409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -1719,7 +2444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1754,7 +2479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1789,7 +2514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1824,7 +2549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -1859,7 +2584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1894,7 +2619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
@@ -1929,7 +2654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1964,7 +2689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
@@ -1999,7 +2724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -2034,7 +2759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
@@ -2069,7 +2794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -2104,7 +2829,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
@@ -2139,7 +2864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -2174,7 +2899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>52</v>
       </c>
@@ -2209,7 +2934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>54</v>
       </c>
@@ -2244,7 +2969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>56</v>
       </c>
@@ -2279,7 +3004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
@@ -2314,7 +3039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>60</v>
       </c>
@@ -2349,7 +3074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
@@ -2384,7 +3109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>64</v>
       </c>
@@ -2419,7 +3144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
@@ -2454,7 +3179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>68</v>
       </c>
@@ -2489,12 +3214,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -2503,158 +3230,2124 @@
       <c r="K29" s="8"/>
       <c r="L29" s="12"/>
     </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="16"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="14">
+        <v>4</v>
+      </c>
+      <c r="G34" s="14">
+        <v>3</v>
+      </c>
+      <c r="H34" s="14">
+        <v>3</v>
+      </c>
+      <c r="I34" s="14"/>
+      <c r="J34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="14">
+        <v>8</v>
+      </c>
+      <c r="G35" s="14">
+        <v>6</v>
+      </c>
+      <c r="H35" s="14">
+        <v>7</v>
+      </c>
+      <c r="I35" s="14">
+        <v>0.33</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="14">
+        <v>12</v>
+      </c>
+      <c r="G36" s="14">
+        <v>9</v>
+      </c>
+      <c r="H36" s="14">
+        <v>12</v>
+      </c>
+      <c r="I36" s="14"/>
+      <c r="J36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="14"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="14">
+        <v>4</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="14">
+        <v>6</v>
+      </c>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B52" s="14"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="14"/>
+      <c r="C54" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="14"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="14">
+        <v>3</v>
+      </c>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="14"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="14">
+        <v>2</v>
+      </c>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B57" s="14"/>
+      <c r="C57" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="14">
+        <v>3</v>
+      </c>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="14"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" s="14">
+        <v>5</v>
+      </c>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" s="14"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" s="14">
+        <v>4</v>
+      </c>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" s="14">
+        <v>1</v>
+      </c>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="14"/>
+      <c r="C62" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="14"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" s="14"/>
+      <c r="C64" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="14"/>
+      <c r="C65" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="14"/>
+      <c r="C66" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" s="14"/>
+      <c r="C67" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B68" s="14"/>
+      <c r="C68" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" s="14"/>
+      <c r="C69" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" s="14"/>
+      <c r="C70" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" s="14"/>
+      <c r="C71" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" s="14"/>
+      <c r="C72" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" s="14"/>
+      <c r="C73" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B74" s="14"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B75" s="14"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="2"/>
+    </row>
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" s="14"/>
+      <c r="C76" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77" s="15"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="14">
+        <v>7</v>
+      </c>
+      <c r="G77" s="14">
+        <v>6</v>
+      </c>
+      <c r="H77" s="14">
+        <v>7</v>
+      </c>
+      <c r="I77" s="14">
+        <v>0.33</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="14"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="14">
+        <v>3</v>
+      </c>
+      <c r="G78" s="14">
+        <v>3</v>
+      </c>
+      <c r="H78" s="14">
+        <v>3</v>
+      </c>
+      <c r="I78" s="14">
+        <v>0</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" s="14"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="14">
+        <v>12</v>
+      </c>
+      <c r="G79" s="14">
+        <v>12</v>
+      </c>
+      <c r="H79" s="14">
+        <v>9</v>
+      </c>
+      <c r="I79" s="14"/>
+      <c r="J79" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="14"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E80" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="14">
+        <v>3</v>
+      </c>
+      <c r="G80" s="14">
+        <v>2</v>
+      </c>
+      <c r="H80" s="14">
+        <v>3</v>
+      </c>
+      <c r="I80" s="14"/>
+      <c r="J80" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" s="14"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="14">
+        <v>4</v>
+      </c>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L81" s="2"/>
+    </row>
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="14"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="14">
+        <v>6</v>
+      </c>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" s="14"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="14">
+        <v>2</v>
+      </c>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K83" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L83" s="2"/>
+    </row>
+    <row r="84" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B84" s="14"/>
+      <c r="C84" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="15"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="2"/>
+    </row>
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" s="14"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="14">
+        <v>3</v>
+      </c>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L85" s="2"/>
+    </row>
+    <row r="86" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B86" s="14"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="2"/>
+    </row>
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" s="14"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F87" s="14">
+        <v>8</v>
+      </c>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K87" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L87" s="2"/>
+    </row>
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="14"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="14">
+        <v>5</v>
+      </c>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K88" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L88" s="2"/>
+    </row>
+    <row r="89" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B89" s="14"/>
+      <c r="C89" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="13"/>
+      <c r="L89" s="2"/>
+    </row>
+    <row r="90" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D90" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="13"/>
+      <c r="L90" s="2"/>
+    </row>
+    <row r="91" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B91" s="14"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="13"/>
+      <c r="L91" s="2"/>
+    </row>
+    <row r="92" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B92" s="14"/>
+      <c r="C92" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="13"/>
+      <c r="L92" s="2"/>
+    </row>
+    <row r="93" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B93" s="14"/>
+      <c r="C93" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="13"/>
+      <c r="L93" s="2"/>
+    </row>
+    <row r="94" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B94" s="14"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E94" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="13"/>
+      <c r="L94" s="2"/>
+    </row>
+    <row r="95" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B95" s="14"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="13"/>
+      <c r="L95" s="2"/>
+    </row>
+    <row r="96" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B96" s="14"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F96" s="14"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="13"/>
+      <c r="L96" s="2"/>
+    </row>
+    <row r="97" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B97" s="14"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="14"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="15"/>
+      <c r="K97" s="13"/>
+      <c r="L97" s="2"/>
+    </row>
+    <row r="98" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B98" s="14"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F98" s="14"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="13"/>
+      <c r="L98" s="2"/>
+    </row>
+    <row r="99" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B99" s="14"/>
+      <c r="C99" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D99" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F99" s="14"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="14"/>
+      <c r="I99" s="14"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="2"/>
+    </row>
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B100" s="14"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="14">
+        <v>9</v>
+      </c>
+      <c r="G100" s="14"/>
+      <c r="H100" s="14"/>
+      <c r="I100" s="14"/>
+      <c r="J100" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L100" s="2"/>
+    </row>
+    <row r="101" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B101" s="14"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="15"/>
+      <c r="K101" s="13"/>
+      <c r="L101" s="2"/>
+    </row>
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B102" s="14"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="14">
+        <v>2</v>
+      </c>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K102" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L102" s="2"/>
+    </row>
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B103" s="14"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" s="14">
+        <v>4</v>
+      </c>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
+      <c r="I103" s="14"/>
+      <c r="J103" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K103" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L103" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="14"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E104" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F104" s="14">
+        <v>3</v>
+      </c>
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="14"/>
+      <c r="J104" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K104" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L104" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="14"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" s="14">
+        <v>4</v>
+      </c>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
+      <c r="I105" s="14"/>
+      <c r="J105" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K105" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L105" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B106" s="14"/>
+      <c r="C106" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="D106" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E106" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F106" s="14"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="14"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="15"/>
+      <c r="K106" s="13"/>
+      <c r="L106" s="2"/>
+    </row>
+    <row r="107" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B107" s="14"/>
+      <c r="C107" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E107" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="14"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="15"/>
+      <c r="K107" s="13"/>
+      <c r="L107" s="2"/>
+    </row>
+    <row r="108" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B108" s="14"/>
+      <c r="C108" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D108" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E108" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F108" s="14"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="15"/>
+      <c r="K108" s="13"/>
+      <c r="L108" s="2"/>
+    </row>
+    <row r="109" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B109" s="10"/>
+      <c r="C109" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F109" s="10"/>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+      <c r="J109" s="11"/>
+      <c r="K109" s="8"/>
+      <c r="L109" s="17"/>
+    </row>
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="B110" s="20"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E110" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F110" s="21">
+        <v>2</v>
+      </c>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="21"/>
+      <c r="J110" s="22"/>
+      <c r="K110" s="19"/>
+      <c r="L110" s="12"/>
+    </row>
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B111" s="20"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E111" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F111" s="21">
+        <v>1</v>
+      </c>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+      <c r="I111" s="21"/>
+      <c r="J111" s="22"/>
+      <c r="K111" s="19"/>
+      <c r="L111" s="12"/>
+    </row>
+    <row r="112" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B112" s="20"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E112" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F112" s="21">
+        <v>7</v>
+      </c>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21"/>
+      <c r="I112" s="21"/>
+      <c r="J112" s="22"/>
+      <c r="K112" s="19"/>
+      <c r="L112" s="12"/>
+    </row>
+    <row r="113" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B113" s="20"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E113" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F113" s="21">
+        <v>5</v>
+      </c>
+      <c r="G113" s="21"/>
+      <c r="H113" s="21"/>
+      <c r="I113" s="21"/>
+      <c r="J113" s="22"/>
+      <c r="K113" s="19"/>
+      <c r="L113" s="12"/>
+    </row>
+    <row r="114" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B114" s="20"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E114" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114" s="21"/>
+      <c r="G114" s="21"/>
+      <c r="H114" s="21"/>
+      <c r="I114" s="21"/>
+      <c r="J114" s="22"/>
+      <c r="K114" s="19"/>
+      <c r="L114" s="12"/>
+    </row>
+    <row r="115" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B115" s="20"/>
+      <c r="C115" s="19"/>
+      <c r="D115" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E115" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F115" s="21"/>
+      <c r="G115" s="21"/>
+      <c r="H115" s="21"/>
+      <c r="I115" s="21"/>
+      <c r="J115" s="22"/>
+      <c r="K115" s="19"/>
+      <c r="L115" s="12"/>
+    </row>
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B116" s="20"/>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E116" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F116" s="21">
+        <v>0</v>
+      </c>
+      <c r="G116" s="21">
+        <v>0</v>
+      </c>
+      <c r="H116" s="21">
+        <v>0</v>
+      </c>
+      <c r="I116" s="21"/>
+      <c r="J116" s="22"/>
+      <c r="K116" s="19"/>
+      <c r="L116" s="12"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D99 D111:D113">
-    <cfRule type="cellIs" dxfId="52" priority="40" operator="equal">
+  <conditionalFormatting sqref="D111:D113">
+    <cfRule type="cellIs" dxfId="90" priority="46" operator="equal">
       <formula>"Temple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="47" operator="equal">
       <formula>"Neutral"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="48" operator="equal">
       <formula>"Citadel"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E99 E111:E113">
-    <cfRule type="cellIs" dxfId="49" priority="37" operator="equal">
+  <conditionalFormatting sqref="E111:E113">
+    <cfRule type="cellIs" dxfId="87" priority="43" operator="equal">
       <formula>"Boon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="44" operator="equal">
       <formula>"Spell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="45" operator="equal">
       <formula>"Creature"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D28">
-    <cfRule type="cellIs" dxfId="46" priority="34" operator="equal">
+  <conditionalFormatting sqref="D2:D116">
+    <cfRule type="cellIs" dxfId="84" priority="40" operator="equal">
       <formula>"Temple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="41" operator="equal">
       <formula>"Neutral"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="42" operator="equal">
       <formula>"Citadel"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E28">
-    <cfRule type="cellIs" dxfId="43" priority="31" operator="equal">
+  <conditionalFormatting sqref="E2:E116">
+    <cfRule type="cellIs" dxfId="81" priority="37" operator="equal">
       <formula>"Boon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="38" operator="equal">
       <formula>"Spell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="39" operator="equal">
       <formula>"Creature"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E110">
-    <cfRule type="cellIs" dxfId="40" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="34" operator="equal">
       <formula>"Temple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="35" operator="equal">
       <formula>"Neutral"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="36" operator="equal">
       <formula>"Citadel"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F110">
-    <cfRule type="cellIs" dxfId="37" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="31" operator="equal">
       <formula>"Boon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="32" operator="equal">
       <formula>"Spell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="33" operator="equal">
       <formula>"Creature"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H103">
-    <cfRule type="cellIs" dxfId="34" priority="22" operator="equal">
+  <conditionalFormatting sqref="A110:A111">
+    <cfRule type="cellIs" dxfId="72" priority="22" operator="equal">
       <formula>"Temple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="23" operator="equal">
       <formula>"Neutral"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
       <formula>"Citadel"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I103">
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
+  <conditionalFormatting sqref="B110:B111">
+    <cfRule type="cellIs" dxfId="69" priority="19" operator="equal">
       <formula>"Boon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="20" operator="equal">
       <formula>"Spell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="21" operator="equal">
       <formula>"Creature"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A97 A109:A111">
-    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
+  <conditionalFormatting sqref="D30:D109">
+    <cfRule type="cellIs" dxfId="66" priority="4" operator="equal">
       <formula>"Temple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="5" operator="equal">
       <formula>"Neutral"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="6" operator="equal">
       <formula>"Citadel"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B97 B109:B111">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+  <conditionalFormatting sqref="E30:E109">
+    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
       <formula>"Boon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="2" operator="equal">
       <formula>"Spell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
-      <formula>"Creature"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B108">
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
-      <formula>"Temple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
-      <formula>"Neutral"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
-      <formula>"Citadel"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
-      <formula>"Boon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
-      <formula>"Spell"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
-      <formula>"Creature"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E101">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
-      <formula>"Temple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
-      <formula>"Neutral"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
-      <formula>"Citadel"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F101">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
-      <formula>"Boon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
-      <formula>"Spell"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
       <formula>"Creature"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2667,13 +5360,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>